<commit_message>
fix: tracing method option for not ok
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/tracing.xlsx
+++ b/config/itech-aurum/forms/app/tracing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC0872E-BD12-1C42-820C-D1CEE587B96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30129F8D-6DAD-AA48-942F-B029091FE9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-2900" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-2400" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -263,9 +263,6 @@
     <t>How was the client traced?</t>
   </si>
   <si>
-    <t>selected(${client_ok}, 'yes_ok') or selected(${client_ok}, 'yes_not_ok')</t>
-  </si>
-  <si>
     <t>Trace Person</t>
   </si>
   <si>
@@ -297,6 +294,18 @@
   </si>
   <si>
     <t>client_traced</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>if(${trace_medium}='sms_phone', "Traced by SMS/Phone ", "Traced by home visit")</t>
+  </si>
+  <si>
+    <t>&lt;h4 style="color: #337ab7;"&gt;Complete this task to demonstrate follow-up after no contact or after incomplete referral to care for minor and adult VMMC clients. 
+&lt;p&gt;This task is triggered for the Hub Nurse and the Site Nurse at the Clinic where the client is enrolled.&lt;/p&gt;
+This form should appear on the persons profile (As an action form) as well and if completed, it should clear the tracing task
+&lt;/h4&gt;</t>
   </si>
   <si>
     <t>if(
@@ -306,7 +315,7 @@
            ${client_ok}='yes_ok', 
            "Client successfully traced and reports no concerns (no follow-up needed)", 
             if(
-                   ${client_ok}='yes_not_ok',
+                   ${client_ok}='not_ok',
                   "Client successfully traced and reports a potential AE",
                   if( ${client_ok}='yes_visited', "Client already reviewed by site team ", "")
              )
@@ -314,16 +323,7 @@
 )</t>
   </si>
   <si>
-    <t>method</t>
-  </si>
-  <si>
-    <t>if(${trace_medium}='sms_phone', "Traced by SMS/Phone ", "Traced by home visit")</t>
-  </si>
-  <si>
-    <t>&lt;h4 style="color: #337ab7;"&gt;Complete this task to demonstrate follow-up after no contact or after incomplete referral to care for minor and adult VMMC clients. 
-&lt;p&gt;This task is triggered for the Hub Nurse and the Site Nurse at the Clinic where the client is enrolled.&lt;/p&gt;
-This form should appear on the persons profile (As an action form) as well and if completed, it should clear the tracing task
-&lt;/h4&gt;</t>
+    <t>selected(${client_ok}, 'yes_ok') or selected(${client_ok}, 'not_ok')</t>
   </si>
 </sst>
 </file>
@@ -759,8 +759,8 @@
   <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1119,7 +1119,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1155,7 +1155,7 @@
         <v>48</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1230,7 +1230,7 @@
         <v>77</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -1295,13 +1295,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>44</v>
       </c>
       <c r="K22" s="27" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1309,13 +1309,13 @@
         <v>19</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>44</v>
       </c>
       <c r="K23" s="24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2343,7 +2343,7 @@
         <v>53</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>72</v>
@@ -2357,7 +2357,7 @@
         <v>49</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2381,10 +2381,10 @@
         <v>76</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2392,10 +2392,10 @@
         <v>76</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3437,13 +3437,13 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="C2" s="25" t="s">
         <v>80</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>81</v>
       </c>
       <c r="D2" t="s">
         <v>62</v>

</xml_diff>